<commit_message>
added recipes to xlsx
</commit_message>
<xml_diff>
--- a/gohan_dousuru.xlsx
+++ b/gohan_dousuru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\81701\gohan_dousuru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B6B3305-F3A5-4ED7-A359-5A5BC0D1C300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8A68BF-15DC-4734-9F6C-B9AD856D8FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24000" yWindow="1695" windowWidth="21600" windowHeight="11295" xr2:uid="{C1E85500-B634-403D-917B-8BEEE78295ED}"/>
+    <workbookView xWindow="-28815" yWindow="0" windowWidth="26415" windowHeight="15585" xr2:uid="{C1E85500-B634-403D-917B-8BEEE78295ED}"/>
   </bookViews>
   <sheets>
     <sheet name="gohan_dousuru" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>menu</t>
   </si>
@@ -182,6 +182,120 @@
   </si>
   <si>
     <t>ポトフ</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/17631433-%E5%B1%85%E9%85%92%E5%B1%8B%E9%A2%A8%E3%82%84%E3%81%BF%E3%81%A4%E3%81%8D%E3%81%8D%E3%82%85%E3%81%86%E3%82%8A</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19223790-%E8%B1%9A%E3%81%B0%E3%82%89%E3%81%8C%E6%9C%80%E9%AB%98-%E8%82%89%E8%B1%86%E8%85%90</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/20870681-%E6%AE%8B%E3%82%8A%E7%89%A9%E3%81%A7%E3%82%82%E7%B5%B6%E5%93%81%E8%B1%9A%E3%82%AD%E3%83%A0%E3%83%81%E3%83%81%E3%83%A3%E3%83%BC%E3%83%8F%E3%83%B3</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/21881392-%E3%82%A2%E3%82%B9%E3%83%91%E3%83%A9%E3%81%AE%E8%B1%9A%E3%83%90%E3%83%A9%E5%B7%BB%E3%81%8D%E3%82%93%E3%81%93</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/21679786-%E7%8E%89%E3%81%AD%E3%81%8E%E5%A4%A7%E9%87%8F%E6%B6%88%E8%B2%BB%E5%AD%90%E4%BE%9B%E3%81%AB%E3%82%82%E7%8E%89%E3%81%AD%E3%81%8E%E7%84%BC%E3%81%8D</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/24032001-%E7%B0%A1%E5%8D%98%E3%81%94%E9%A3%AF%E3%81%8C%E3%81%99%E3%81%99%E3%82%80%E7%94%98%E8%BE%9B%E3%83%94%E3%83%BC%E3%83%9E%E3%83%B3%E3%81%9D%E3%81%BC%E3%82%8D</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/17927474-%E9%BB%92%E8%B1%86%E3%81%A8%E7%89%9B%E8%82%89%E3%81%AE%E7%85%AE%E8%BE%BC%E3%81%BF%E3%83%95%E3%82%A7%E3%82%B8%E3%83%A7%E3%82%A2%E3%83%BC%E3%83%80%E9%A2%A8</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18642166-%E3%83%90%E3%82%BF%E3%83%BC%E9%86%A4%E6%B2%B9%E3%81%AE%E7%84%BC%E3%81%8D%E3%81%A8%E3%81%86%E3%82%82%E3%82%8D%E3%81%93%E3%81%97</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/21608458-%E3%82%93%E3%82%BF%E3%83%AC%E3%81%8C%E3%81%9F%E3%81%BE%E3%82%89%E3%82%93%E6%97%A8%E3%81%84%E7%89%9B%E3%81%A8%E3%82%A2%E3%82%B9%E3%83%91%E3%83%A9</t>
+  </si>
+  <si>
+    <t>牛肉とアスパラの炒め物</t>
+  </si>
+  <si>
+    <t>焼きとうもろこし</t>
+  </si>
+  <si>
+    <t>ツナ炒飯</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18251479-%E3%82%B7%E3%82%A7%E3%83%95%E3%83%91%E3%83%91%E3%81%AE%E3%81%82%E3%82%8A%E5%90%88%E3%82%8F%E3%81%9B%E3%83%84%E3%83%8A%E3%83%81%E3%83%A3%E3%83%BC%E3%83%8F%E3%83%B3</t>
+  </si>
+  <si>
+    <t>海老の生春巻き</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18098787-%E3%82%A8%E3%83%93%E3%81%AE%E7%94%9F%E6%98%A5%E5%B7%BB%E3%81%8D</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/21637659-%E8%89%B2%E3%82%93%E3%81%AA%E9%87%8E%E8%8F%9C%E3%81%A7%E3%81%BB%E3%81%A3%E3%81%93%E3%82%8A%E3%83%9D%E3%83%88%E3%83%95%E4%BD%99%E3%82%8A%E9%87%8E%E8%8F%9C%E3%81%A7</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19563335-%E3%81%A8%E3%81%A6%E3%82%82%E7%B0%A1%E5%8D%98%E3%83%88%E3%83%9E%E3%83%88%E7%BC%B6%E3%81%A7%E7%B5%B6%E5%93%81%E3%83%A9%E3%82%BF%E3%83%88%E3%82%A5%E3%82%A4%E3%83%A6</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18714519-%E3%81%98%E3%82%85%E3%82%8F%E3%81%AA%E3%81%99%E3%81%AE%E7%85%AE%E6%B5%B8%E3%81%97</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/21599735-%E6%88%91%E3%81%8C%E5%AE%B6%E8%87%AA%E6%85%A2%E3%81%AE%E7%94%9F%E5%A7%9C%E7%84%BC%E3%81%8D%E3%81%8A%E8%82%89%E6%9F%94%E3%82%89%E3%81%8B%E3%81%84</t>
+  </si>
+  <si>
+    <t>玉ねぎ,キャベツ</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19040237-%E3%83%AC%E3%82%BF%E3%82%B9%E3%81%A8%E3%82%B8%E3%83%A3%E3%83%90%E3%83%B3%E9%9F%93%E5%9B%BD%E3%81%AE%E3%82%8A%E3%81%AE%E7%B0%A1%E5%8D%98%E3%82%B5%E3%83%A9%E3%83%80</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19913495-%E3%82%B7%E3%83%B3%E3%83%97%E3%83%AB%E3%83%AD%E3%83%BC%E3%83%AB%E3%82%AD%E3%83%A3%E3%83%99%E3%83%84%E3%82%B3%E3%83%B3%E3%82%BD%E3%83%A1%E3%82%B9%E3%83%BC%E3%83%97</t>
+  </si>
+  <si>
+    <t>ガレット</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/21493625-%E3%81%98%E3%82%83%E3%81%8C%E3%81%84%E3%82%82%E3%81%A7%E7%B0%A1%E5%8D%98%E3%83%91%E3%83%AA%E3%83%91%E3%83%AA%E7%84%BC%E3%81%8D</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19326362-%E3%83%AC%E3%83%B3%E3%82%B8%E3%81%AB%E3%81%8A%E4%BB%BB%E3%81%9B%E3%81%A7%E3%82%82%E6%9C%AC%E6%A0%BC%E7%9A%84-%E3%81%8B%E3%81%BC%E3%81%A1%E3%82%83%E3%81%AE%E7%85%AE%E7%89%A9</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18442207-%E8%A6%AA%E5%AD%90%E4%B8%BC</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18949184-%E3%81%8D%E3%82%93%E3%81%B4%E3%82%89%E3%81%94%E3%81%BC%E3%81%86</t>
+  </si>
+  <si>
+    <t>コロッケ</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/20388518-%E7%AF%80%E7%B4%84%E7%B0%A1%E5%8D%98%E3%81%8A%E3%81%84%E3%81%97%E3%81%84%E8%82%89%E3%81%AA%E3%81%97%E3%82%B3%E3%83%AD%E3%83%83%E3%82%B1</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19559616-%E6%88%91%E3%81%8C%E5%AE%B6%E3%81%AE%E7%89%9B%E7%9A%BF</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/20601981-%E3%83%94%E3%83%BC%E3%83%9E%E3%83%B3%E3%81%AE%E8%82%89%E8%A9%B0%E3%82%81%E6%97%A8%E3%81%BF%E6%BA%A2%E3%82%8C%E3%82%8B%E7%BE%8E%E5%91%B3%E3%81%97%E3%81%95</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/19780969-%E7%B0%A1%E5%8D%98%E6%9C%AC%E6%A0%BC%E9%BA%BB%E5%A9%86%E8%8C%84%E5%AD%90</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18194204-%E8%B1%9A%E6%B1%81</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/18623215-%E8%B6%85%E3%81%8B%E3%82%93%E3%81%9F%E3%82%93%E3%81%A7%E7%BE%8E%E5%91%B3%E3%81%97%E3%81%84%E3%82%AD%E3%83%BC%E3%83%9E%E3%82%AB%E3%83%AC%E3%83%BC</t>
+  </si>
+  <si>
+    <t>https://cookpad.com/jp/recipes/20351441-%E3%83%93%E3%83%BC%E3%83%95%E3%82%B7%E3%83%81%E3%83%A5%E3%83%BC</t>
+  </si>
+  <si>
+    <t>https://www.hijiki.org/recipe/%E3%81%B2%E3%81%98%E3%81%8D%E5%85%A5%E3%82%8A%E8%82%89%E3%81%98%E3%82%83%E3%81%8C/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_bM8TneFoqs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=foPvVxVqkWM</t>
   </si>
 </sst>
 </file>
@@ -1042,13 +1156,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B76ECC5-F523-4AD3-9CB8-95B1825D6B57}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1074,6 +1192,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1085,6 +1206,9 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1093,6 +1217,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1109,6 +1236,9 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1117,6 +1247,9 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1128,6 +1261,9 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1137,7 +1273,10 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,6 +1308,9 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1177,6 +1319,9 @@
       <c r="B13" t="s">
         <v>5</v>
       </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1210,16 +1355,22 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1229,8 +1380,11 @@
       <c r="C18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1238,7 +1392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1246,7 +1400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1257,7 +1411,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1268,7 +1422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1279,7 +1433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1289,16 +1443,22 @@
       <c r="C24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1308,16 +1468,22 @@
       <c r="C26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1325,23 +1491,29 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1351,8 +1523,11 @@
       <c r="C31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1362,16 +1537,22 @@
       <c r="C32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1381,8 +1562,11 @@
       <c r="C34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1390,7 +1574,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1401,31 +1585,111 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" t="s">
         <v>49</v>
       </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D16" r:id="rId1" xr:uid="{D33CC9DC-F2F5-430B-8BC2-35957C57558D}"/>
+    <hyperlink ref="D26" r:id="rId2" xr:uid="{68FBDA6C-39C8-4A77-84CD-D7AD18C0140D}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{196CD9BD-3980-47FD-8D55-311FA292D7AB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>